<commit_message>
Adding Callaway Edge clubs to tracking sheets.
</commit_message>
<xml_diff>
--- a/Data_Sets/Tee_Shot_Range_Data.xlsx
+++ b/Data_Sets/Tee_Shot_Range_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanwenger/Desktop/Desktop_Master/Coding/github_projects/Golf_Caddie/Golf_Caddie/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanwenger/Desktop/Desktop_Master/Coding/github_projects/Golf_Caddie/Golf_Caddie/Data_Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACBB013-DBC3-7A40-85C4-243DFE1434FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD628C8-9EF0-2147-935E-FE53B5E90427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="1420" windowWidth="26440" windowHeight="14400" xr2:uid="{D346C99F-FB13-B94F-B1D1-A02BA65BDF1C}"/>
+    <workbookView xWindow="6860" yWindow="500" windowWidth="21880" windowHeight="14060" xr2:uid="{D346C99F-FB13-B94F-B1D1-A02BA65BDF1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,19 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>PW</t>
-  </si>
-  <si>
-    <t>SW</t>
-  </si>
-  <si>
-    <t>HW</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>3 Wood</t>
   </si>
@@ -60,6 +48,57 @@
   </si>
   <si>
     <t>Driver</t>
+  </si>
+  <si>
+    <t>CE-6</t>
+  </si>
+  <si>
+    <t>CE-7</t>
+  </si>
+  <si>
+    <t>CE-8</t>
+  </si>
+  <si>
+    <t>CE-9</t>
+  </si>
+  <si>
+    <t>CE-PW</t>
+  </si>
+  <si>
+    <t>CE-SW</t>
+  </si>
+  <si>
+    <t>P-3</t>
+  </si>
+  <si>
+    <t>P-4</t>
+  </si>
+  <si>
+    <t>P-5</t>
+  </si>
+  <si>
+    <t>P-6</t>
+  </si>
+  <si>
+    <t>P-7</t>
+  </si>
+  <si>
+    <t>P-8</t>
+  </si>
+  <si>
+    <t>P-9</t>
+  </si>
+  <si>
+    <t>P-W</t>
+  </si>
+  <si>
+    <t>PM-PW</t>
+  </si>
+  <si>
+    <t>PM-SW</t>
+  </si>
+  <si>
+    <t>PM-LW</t>
   </si>
 </sst>
 </file>
@@ -83,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -106,14 +145,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,97 +547,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212046D1-1FE3-AA46-B1AD-4FA0A036A147}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="M1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="O1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1">
+      <c r="P1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1">
+      <c r="Q1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1">
+      <c r="R1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1">
+      <c r="S1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1">
+      <c r="T1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D2">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B2">
         <f>AVERAGE([1]Sheet1!$H$40)</f>
         <v>123</v>
       </c>
-      <c r="E2">
+      <c r="C2">
         <f>AVERAGE([1]Sheet1!$H$49)</f>
         <v>142</v>
       </c>
-      <c r="F2">
+      <c r="D2">
         <f>AVERAGE([1]Sheet1!$F$40,[1]Sheet1!$F$49)</f>
         <v>130.5</v>
       </c>
-      <c r="G2">
+      <c r="E2">
         <f>AVERAGE([1]Sheet1!$B$49,[1]Sheet1!$C$49)</f>
         <v>123</v>
       </c>
-      <c r="H2">
+      <c r="F2">
         <f>AVERAGE([1]Sheet1!$C$40)</f>
         <v>100</v>
       </c>
-      <c r="I2">
+      <c r="G2">
         <f>AVERAGE([1]Sheet1!$B$40,[1]Sheet1!$I$40,[1]Sheet1!$I$49)</f>
         <v>107</v>
       </c>
-      <c r="J2">
+      <c r="H2">
         <f>AVERAGE([1]Sheet1!$G$40,[1]Sheet1!$E$49,[1]Sheet1!$G$49)</f>
         <v>95</v>
       </c>
-      <c r="K2">
+      <c r="I2">
         <f>AVERAGE([1]Sheet1!$D$40,[1]Sheet1!$J$40,[1]Sheet1!$D$49,[1]Sheet1!$J$49)</f>
         <v>71.25</v>
       </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>